<commit_message>
add def menu e loop
</commit_message>
<xml_diff>
--- a/Clientes 2.xlsx
+++ b/Clientes 2.xlsx
@@ -788,13 +788,64 @@
       </c>
     </row>
     <row r="21">
-      <c r="C21" s="5" t="n"/>
+      <c r="C21" s="5" t="n">
+        <v>110</v>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>marcos paulo</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>11 111111</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>rua macos</t>
+        </is>
+      </c>
     </row>
     <row r="22">
-      <c r="C22" s="5" t="n"/>
+      <c r="C22" s="5" t="n">
+        <v>111</v>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>ana</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>11 2222</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>rua da ana</t>
+        </is>
+      </c>
     </row>
     <row r="23">
-      <c r="C23" s="5" t="n"/>
+      <c r="C23" s="5" t="n">
+        <v>112</v>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>julio</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>11 899</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>rua do jolio</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="C24" s="5" t="n"/>

</xml_diff>